<commit_message>
Update file báo cáo
</commit_message>
<xml_diff>
--- a/KeHoach.xlsx
+++ b/KeHoach.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNTT_K20\Project1\Final_Project\Final-Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4951f0d6c4070b2d/Desktop/Final-Project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDDCDD6-F295-4E1D-A938-005D5DD80605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{AEDDCDD6-F295-4E1D-A938-005D5DD80605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7372C37B-BD02-49EF-9AC8-6778812B0282}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>STT</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Thiết kế database</t>
+  </si>
+  <si>
+    <t>Làm ppt</t>
+  </si>
+  <si>
+    <t>Viết báo cáo</t>
   </si>
 </sst>
 </file>
@@ -273,23 +279,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -320,20 +340,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="dd/mm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -502,9 +508,9 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Phan Hồng Sơn" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ngày bắt đầu dự kiến" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ngày kết thúc dự kiến" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ngày bắt đầu thực tế" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Ngày kết thúc thực tế" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ghi chú" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ngày bắt đầu thực tế" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Ngày kết thúc thực tế" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ghi chú" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -810,7 +816,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,65 +833,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" s="11" customFormat="1" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -1080,9 +1086,9 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -1103,7 +1109,7 @@
       <c r="I14" s="9">
         <v>44844</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
@@ -1201,7 +1207,9 @@
       <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="E18" s="12" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1382,9 @@
       <c r="D25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="F25" s="9">
         <v>44882</v>
       </c>
@@ -1420,7 +1430,9 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12" t="s">
         <v>34</v>
@@ -1474,7 +1486,9 @@
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D29" s="12" t="s">
         <v>34</v>
       </c>

</xml_diff>